<commit_message>
Uploaded 22-Feb-2024 09:51:18 {/src/main/resources/com/myspace/insect/price_tnds.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/myspace/insect/price_tnds.xlsx
+++ b/src/main/resources/com/myspace/insect/price_tnds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\SG2PEPF000DE4F3\EXCELCNV\d0b4e16f-6411-4fc1-a9ca-450df9bea49a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\SG2PEPF000DE510\EXCELCNV\ec5407ed-4199-41b2-989f-f43ae50305f1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{335FD5F8-3DE4-4BF1-B289-168CAFB6A457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D940A8F6-3D74-4E08-A534-B0C97AD72B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" tabRatio="259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <t>RuleSet</t>
   </si>
   <si>
-    <t>com.finos.insurance.hdi.pricing</t>
+    <t>com.myspace.insect</t>
   </si>
   <si>
     <t>Functions</t>
@@ -830,7 +830,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1"/>

</xml_diff>